<commit_message>
EPBDS-10335 Fix compilation of Lookup wider 100 columns
EPBDS-8743 Also was fixed compilation of lookups with empty body, so no errors are thrown

--HG--
branch : 5.23.5.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8743_NPE_fix.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8743_NPE_fix.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC12BE7-CF15-4E6A-9DE6-A05B7E56793A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="12270"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Datatype myType &lt;String&gt;</t>
   </si>
@@ -64,17 +68,31 @@
   </si>
   <si>
     <t>Rules Double[] myRules(myType aaa, myType2 bbb)</t>
+  </si>
+  <si>
+    <t>Test myRules</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Arg1</t>
+  </si>
+  <si>
+    <t>Arg2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,14 +116,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,7 +153,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -143,6 +161,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -191,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +245,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,6 +297,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,18 +489,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" width="16" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -457,25 +512,25 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
@@ -496,7 +551,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9"/>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>0</v>
@@ -526,6 +580,41 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
         <v>14</v>
       </c>
     </row>
@@ -536,28 +625,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>